<commit_message>
PROS-5736 - CCRU - New Contract Execution
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/KPIs for DB - Spirits.xlsx
+++ b/Projects/CCRU_SAND/Data/KPIs for DB - Spirits.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">KPI Level 3 Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Weight</t>
+    <t xml:space="preserve">KPI Level 2 Weight</t>
   </si>
   <si>
     <t xml:space="preserve">Spirits 2018 - MT - Convenience</t>
@@ -267,15 +267,15 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.3348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.9860465116279"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.6186046511628"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>